<commit_message>
actualizado del 717 al 722
</commit_message>
<xml_diff>
--- a/normativa/Anexos/L03T07C02/L03T07C02A01.xlsx
+++ b/normativa/Anexos/L03T07C02/L03T07C02A01.xlsx
@@ -20,9 +20,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>Entidad Financiera:</t>
-  </si>
-  <si>
     <t>Gerente General</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>LIBRO 3°, TÍTULO VII, CAPÍTULO II</t>
+  </si>
+  <si>
+    <t>Entidad Supervisada:</t>
   </si>
 </sst>
 </file>
@@ -503,6 +503,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -516,24 +534,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,8 +847,8 @@
   </sheetPr>
   <dimension ref="A2:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -865,39 +865,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="A2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
+      <c r="A3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -909,7 +909,7 @@
     </row>
     <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -920,46 +920,46 @@
       <c r="H6" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="C8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="E8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="29" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="27" t="s">
+      <c r="H9" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="28"/>
+      <c r="I9" s="34"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -1173,58 +1173,64 @@
     <row r="29" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
       <c r="B38" s="5"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
+        <v>13</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="7"/>
       <c r="H39" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="G8:H8"/>
@@ -1232,25 +1238,19 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D28">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="71" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="68" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Negrita"&amp;8&amp;U
 RECOPILACIÓN DE NORMAS PARA SERVICIOS FINANCIEROS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
     <oddFooter>&amp;L&amp;"Times New Roman,Normal"&amp;9Control de versiones
-Circular ASFI/505/2017 (última)&amp;R&amp;"Times New Roman,Normal"&amp;8Libro 3°
+Circular ASFI/721/2022 (última)&amp;R&amp;"Times New Roman,Normal"&amp;8Libro 3°
 Título VII
 Capítulo II
 Anexo 1

</xml_diff>